<commit_message>
corrected diss data from Nina email, added station location data and script for lat relationships
</commit_message>
<xml_diff>
--- a/raw/crab_diss.xlsx
+++ b/raw/crab_diss.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proj\crab_eval\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1730857A-A3C1-46D0-8D85-A47B94E599E8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9516"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -387,19 +386,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -413,7 +412,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>94</v>
       </c>
@@ -427,7 +426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>99</v>
       </c>
@@ -441,7 +440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>100</v>
       </c>
@@ -455,7 +454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>106</v>
       </c>
@@ -469,12 +468,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>109</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -483,23 +482,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>115</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B8">
         <v>0</v>

</xml_diff>

<commit_message>
added new dissolution data from nina, broke crab_explr
</commit_message>
<xml_diff>
--- a/raw/crab_diss.xlsx
+++ b/raw/crab_diss.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proj\crab_eval\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nina.SCCWRP2K\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9516"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,25 +24,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>stations</t>
+    <t>CTD</t>
   </si>
   <si>
-    <t>no dissolution</t>
-  </si>
-  <si>
-    <t>partial</t>
-  </si>
-  <si>
-    <t>dissolution</t>
+    <t>Outside carapace</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -50,13 +44,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -71,8 +85,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -387,130 +406,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection sqref="A1:B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="C1" s="2"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>94</v>
       </c>
       <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>90</v>
+      </c>
+      <c r="B3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>99</v>
+      </c>
+      <c r="B4">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>100</v>
+      </c>
+      <c r="B5">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>106</v>
+      </c>
+      <c r="B6">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>109</v>
+      </c>
+      <c r="B7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>115</v>
+      </c>
+      <c r="B8">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>128</v>
+      </c>
+      <c r="B9">
         <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>99</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>100</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>106</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>109</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>115</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>127</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>